<commit_message>
did some wing length but issue with distribution in r?
</commit_message>
<xml_diff>
--- a/lifehist/2017_10_21 Life history descriptive info.xlsx
+++ b/lifehist/2017_10_21 Life history descriptive info.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21765" windowHeight="10245" firstSheet="3" activeTab="10"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21765" windowHeight="10245" firstSheet="5" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -23,6 +23,7 @@
     <sheet name="AdRate" sheetId="9" r:id="rId9"/>
     <sheet name="LarvRate" sheetId="10" r:id="rId10"/>
     <sheet name="AL" sheetId="11" r:id="rId11"/>
+    <sheet name="Winglength" sheetId="12" r:id="rId12"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1165" uniqueCount="66">
   <si>
     <t>LOC</t>
   </si>
@@ -4961,6 +4962,1773 @@
                   <a:rPr lang="en-US"/>
                   <a:t>Rate of development (1/larvae life)</a:t>
                 </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446046864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Length of adult life</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Low-latitude (Male)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$5,LarvRate!$M$11,LarvRate!$M$17)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>6.0471072346911401E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.7467924511133704E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.7218452412817999E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$5,LarvRate!$M$11,LarvRate!$M$17)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>6.0471072346911401E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.7467924511133704E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.7218452412817999E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>('Emergence time'!$J$2,'Emergence time'!$J$5,'Emergence time'!$J$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(LarvRate!$L$5,LarvRate!$L$11,LarvRate!$L$17)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.5118280251396597E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4967694491428599E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.5169583258823502E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0193-4DAD-9E52-FA97633BB3FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Mid-latitude (Male)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dkDnDiag">
+              <a:fgClr>
+                <a:srgbClr val="FF0000"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$6,LarvRate!$M$12,LarvRate!$M$18)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.3386488843465297E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.7773359381323702E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.02301661853802E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$6,LarvRate!$M$12,LarvRate!$M$18)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.3386488843465297E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.7773359381323702E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.02301661853802E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>(LarvRate!$L$6,LarvRate!$L$12,LarvRate!$L$18)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.8671279041152302E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8271495819999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.4651995811320806E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0193-4DAD-9E52-FA97633BB3FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>High latitude (Male)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="wdUpDiag">
+              <a:fgClr>
+                <a:srgbClr val="FF0000"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$7,LarvRate!$M$13,LarvRate!$M$19)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>3.96618502329368E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.8922245532348995E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.27034328779662E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$7,LarvRate!$M$13,LarvRate!$M$19)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>3.96618502329368E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.8922245532348995E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.27034328779662E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>(LarvRate!$L$7,LarvRate!$L$13,LarvRate!$L$19)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.35098176031746E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.4391032454545497E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0486927058823498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0193-4DAD-9E52-FA97633BB3FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Low-latitude (Female)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$2,LarvRate!$M$8,LarvRate!$M$14)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.8728236519264799E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.3877821535513902E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.2634341923764499E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$2,LarvRate!$M$8,LarvRate!$M$14)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.8728236519264799E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.3877821535513902E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.2634341923764499E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>('Emergence time'!$J$2,'Emergence time'!$J$5,'Emergence time'!$J$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(LarvRate!$L$2,LarvRate!$L$8,LarvRate!$L$14)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.4819107810457499E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3679833544303802E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.27637919784173E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0193-4DAD-9E52-FA97633BB3FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Mid-latitude (Female)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dkDnDiag">
+              <a:fgClr>
+                <a:srgbClr val="0070C0"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$3,LarvRate!$M$9,LarvRate!$M$15)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.4273258985075099E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.61443501850301E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.06938789877785E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$3,LarvRate!$M$9,LarvRate!$M$15)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.4273258985075099E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.61443501850301E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.06938789877785E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>(LarvRate!$L$3,LarvRate!$L$9,LarvRate!$L$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.7904122240157498E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7357551476000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3208757755434802E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-0193-4DAD-9E52-FA97633BB3FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>High latitude (Female)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="wdUpDiag">
+              <a:fgClr>
+                <a:srgbClr val="0070C0"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$4,LarvRate!$M$10,LarvRate!$M$16)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.3582642893852204E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.2067787176241299E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.31407472371946E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$4,LarvRate!$M$10,LarvRate!$M$16)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.3582642893852204E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.2067787176241299E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.31407472371946E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>(LarvRate!$L$4,LarvRate!$L$10,LarvRate!$L$16)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.2485370818181802E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.1413170684210502E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3593154375000002E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-0193-4DAD-9E52-FA97633BB3FF}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="446046864"/>
+        <c:axId val="446046208"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="446046864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Temperature treatment (C)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446046208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="446046208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="9.0000000000000024E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Adult life (days)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446046864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:noFill/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Body size</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Low-latitude (Male)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$5,LarvRate!$M$11,LarvRate!$M$17)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>6.0471072346911401E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.7467924511133704E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.7218452412817999E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$5,LarvRate!$M$11,LarvRate!$M$17)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>6.0471072346911401E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.7467924511133704E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.7218452412817999E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>('Emergence time'!$J$2,'Emergence time'!$J$5,'Emergence time'!$J$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(LarvRate!$L$5,LarvRate!$L$11,LarvRate!$L$17)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.5118280251396597E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.4967694491428599E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.5169583258823502E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B2D0-4D68-8070-EC2D89E40D2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Mid-latitude (Male)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dkDnDiag">
+              <a:fgClr>
+                <a:srgbClr val="FF0000"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$6,LarvRate!$M$12,LarvRate!$M$18)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.3386488843465297E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.7773359381323702E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.02301661853802E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$6,LarvRate!$M$12,LarvRate!$M$18)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.3386488843465297E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.7773359381323702E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.02301661853802E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>(LarvRate!$L$6,LarvRate!$L$12,LarvRate!$L$18)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.8671279041152302E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.8271495819999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.4651995811320806E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B2D0-4D68-8070-EC2D89E40D2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>High latitude (Male)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="wdUpDiag">
+              <a:fgClr>
+                <a:srgbClr val="FF0000"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$7,LarvRate!$M$13,LarvRate!$M$19)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>3.96618502329368E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.8922245532348995E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.27034328779662E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$7,LarvRate!$M$13,LarvRate!$M$19)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>3.96618502329368E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.8922245532348995E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.27034328779662E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>(LarvRate!$L$7,LarvRate!$L$13,LarvRate!$L$19)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.35098176031746E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.4391032454545497E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0486927058823498E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B2D0-4D68-8070-EC2D89E40D2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Low-latitude (Female)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="0070C0"/>
+            </a:solidFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$2,LarvRate!$M$8,LarvRate!$M$14)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.8728236519264799E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.3877821535513902E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.2634341923764499E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$2,LarvRate!$M$8,LarvRate!$M$14)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.8728236519264799E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.3877821535513902E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>8.2634341923764499E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>('Emergence time'!$J$2,'Emergence time'!$J$5,'Emergence time'!$J$8)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>(LarvRate!$L$2,LarvRate!$L$8,LarvRate!$L$14)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.4819107810457499E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3679833544303802E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7.27637919784173E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B2D0-4D68-8070-EC2D89E40D2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Mid-latitude (Female)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="dkDnDiag">
+              <a:fgClr>
+                <a:srgbClr val="0070C0"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$3,LarvRate!$M$9,LarvRate!$M$15)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.4273258985075099E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.61443501850301E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.06938789877785E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$3,LarvRate!$M$9,LarvRate!$M$15)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.4273258985075099E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>7.61443501850301E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.06938789877785E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>(LarvRate!$L$3,LarvRate!$L$9,LarvRate!$L$15)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.7904122240157498E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7357551476000003E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3208757755434802E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-B2D0-4D68-8070-EC2D89E40D2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>High latitude (Female)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="wdUpDiag">
+              <a:fgClr>
+                <a:srgbClr val="0070C0"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="bg1"/>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$4,LarvRate!$M$10,LarvRate!$M$16)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.3582642893852204E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.2067787176241299E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.31407472371946E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(LarvRate!$M$4,LarvRate!$M$10,LarvRate!$M$16)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>5.3582642893852204E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>6.2067787176241299E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>1.31407472371946E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>(LarvRate!$L$4,LarvRate!$L$10,LarvRate!$L$16)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.2485370818181802E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.1413170684210502E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.3593154375000002E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-B2D0-4D68-8070-EC2D89E40D2E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="446046864"/>
+        <c:axId val="446046208"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="446046864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Temperature treatment (C)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446046208"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="446046208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="9.0000000000000024E-2"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Body</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> size (wing length (mm))</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -6935,6 +8703,92 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>417029</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84FDCC4C-C75F-4470-BEA7-21B594066030}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>417029</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDE54B05-0154-41DA-AD2A-A288666B278E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -8608,8 +10462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P9" sqref="P9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9956,6 +11810,1369 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M43"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q8" sqref="Q8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2">
+        <v>20</v>
+      </c>
+      <c r="E2">
+        <v>2.7389523809523801</v>
+      </c>
+      <c r="F2">
+        <v>0.121703159310575</v>
+      </c>
+      <c r="H2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3">
+        <v>20</v>
+      </c>
+      <c r="E3">
+        <v>2.73818181818182</v>
+      </c>
+      <c r="F3">
+        <v>0.104078280160915</v>
+      </c>
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3">
+        <v>20</v>
+      </c>
+      <c r="L3">
+        <v>2.7385033112582802</v>
+      </c>
+      <c r="M3">
+        <v>0.11137784783772101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4">
+        <v>20</v>
+      </c>
+      <c r="E4">
+        <v>2.7714318181818198</v>
+      </c>
+      <c r="F4">
+        <v>0.12535685113065001</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4">
+        <v>20</v>
+      </c>
+      <c r="L4">
+        <v>2.7811518715241901</v>
+      </c>
+      <c r="M4">
+        <v>0.123948216129286</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>2.8000666413799999</v>
+      </c>
+      <c r="F5">
+        <v>0.119848457692754</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5">
+        <v>20</v>
+      </c>
+      <c r="L5">
+        <v>3.0195538461538498</v>
+      </c>
+      <c r="M5">
+        <v>0.125327075931494</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6">
+        <v>2.7487619047619001</v>
+      </c>
+      <c r="F6">
+        <v>0.120182951902467</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6">
+        <v>20</v>
+      </c>
+      <c r="L6">
+        <v>2.7868235294117598</v>
+      </c>
+      <c r="M6">
+        <v>0.110758084532212</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7">
+        <v>2.7991666666666699</v>
+      </c>
+      <c r="F7">
+        <v>0.13706042033909499</v>
+      </c>
+      <c r="H7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7">
+        <v>20</v>
+      </c>
+      <c r="L7">
+        <v>2.8254942339789899</v>
+      </c>
+      <c r="M7">
+        <v>0.13056743316289399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8">
+        <v>3.0195538461538498</v>
+      </c>
+      <c r="F8">
+        <v>0.125327075931494</v>
+      </c>
+      <c r="H8">
+        <v>6</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8">
+        <v>20</v>
+      </c>
+      <c r="L8">
+        <v>2.9781290322580598</v>
+      </c>
+      <c r="M8">
+        <v>0.13290690491023599</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9">
+        <v>2.7722318840579701</v>
+      </c>
+      <c r="F9">
+        <v>0.11069182776141499</v>
+      </c>
+      <c r="H9">
+        <v>7</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9">
+        <v>24</v>
+      </c>
+      <c r="L9">
+        <v>2.5735324675324698</v>
+      </c>
+      <c r="M9">
+        <v>0.124895311394186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>2.7967920792079202</v>
+      </c>
+      <c r="F10">
+        <v>0.110239404645679</v>
+      </c>
+      <c r="H10">
+        <v>8</v>
+      </c>
+      <c r="I10">
+        <v>2</v>
+      </c>
+      <c r="J10" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10">
+        <v>24</v>
+      </c>
+      <c r="L10">
+        <v>2.6305473708223102</v>
+      </c>
+      <c r="M10">
+        <v>0.12098601546047601</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+      <c r="E11">
+        <v>2.8350444444444398</v>
+      </c>
+      <c r="F11">
+        <v>0.13882151754261299</v>
+      </c>
+      <c r="H11">
+        <v>9</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11">
+        <v>24</v>
+      </c>
+      <c r="L11">
+        <v>2.76981818181818</v>
+      </c>
+      <c r="M11">
+        <v>0.109572585600375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>20</v>
+      </c>
+      <c r="E12">
+        <v>2.8131321328068202</v>
+      </c>
+      <c r="F12">
+        <v>0.114780209983717</v>
+      </c>
+      <c r="H12">
+        <v>10</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12">
+        <v>24</v>
+      </c>
+      <c r="L12">
+        <v>2.6306227544910201</v>
+      </c>
+      <c r="M12">
+        <v>0.125667069076184</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>20</v>
+      </c>
+      <c r="E13">
+        <v>2.8090212765957401</v>
+      </c>
+      <c r="F13">
+        <v>0.13301658761576901</v>
+      </c>
+      <c r="H13">
+        <v>11</v>
+      </c>
+      <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13">
+        <v>24</v>
+      </c>
+      <c r="L13">
+        <v>2.7020504477242802</v>
+      </c>
+      <c r="M13">
+        <v>0.14567084051402701</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>20</v>
+      </c>
+      <c r="E14">
+        <v>2.9026153846153799</v>
+      </c>
+      <c r="F14">
+        <v>0.14530917524456699</v>
+      </c>
+      <c r="H14">
+        <v>12</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14">
+        <v>24</v>
+      </c>
+      <c r="L14">
+        <v>2.7746825396825399</v>
+      </c>
+      <c r="M14">
+        <v>0.118603272733611</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <v>20</v>
+      </c>
+      <c r="E15">
+        <v>2.9781290322580598</v>
+      </c>
+      <c r="F15">
+        <v>0.13290690491023599</v>
+      </c>
+      <c r="H15">
+        <v>13</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
+      </c>
+      <c r="J15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15">
+        <v>28</v>
+      </c>
+      <c r="L15">
+        <v>2.4936471014492798</v>
+      </c>
+      <c r="M15">
+        <v>0.114591598010512</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <v>24</v>
+      </c>
+      <c r="E16">
+        <v>2.6098035714285701</v>
+      </c>
+      <c r="F16">
+        <v>0.121065935400036</v>
+      </c>
+      <c r="H16">
+        <v>14</v>
+      </c>
+      <c r="I16">
+        <v>2</v>
+      </c>
+      <c r="J16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16">
+        <v>28</v>
+      </c>
+      <c r="L16">
+        <v>2.48998858068156</v>
+      </c>
+      <c r="M16">
+        <v>0.137612043011724</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17">
+        <v>24</v>
+      </c>
+      <c r="E17">
+        <v>2.5528061224489802</v>
+      </c>
+      <c r="F17">
+        <v>0.122882783655117</v>
+      </c>
+      <c r="H17">
+        <v>15</v>
+      </c>
+      <c r="I17">
+        <v>3</v>
+      </c>
+      <c r="J17" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17">
+        <v>28</v>
+      </c>
+      <c r="L17">
+        <v>2.6284375</v>
+      </c>
+      <c r="M17">
+        <v>0.106593913991372</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="D18">
+        <v>24</v>
+      </c>
+      <c r="E18">
+        <v>2.6240526315789499</v>
+      </c>
+      <c r="F18">
+        <v>0.10878021648406599</v>
+      </c>
+      <c r="H18">
+        <v>16</v>
+      </c>
+      <c r="I18">
+        <v>1</v>
+      </c>
+      <c r="J18" t="s">
+        <v>15</v>
+      </c>
+      <c r="K18">
+        <v>28</v>
+      </c>
+      <c r="L18">
+        <v>2.57161445783133</v>
+      </c>
+      <c r="M18">
+        <v>0.128752083250017</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>14</v>
+      </c>
+      <c r="D19">
+        <v>24</v>
+      </c>
+      <c r="E19">
+        <v>2.6090687631808498</v>
+      </c>
+      <c r="F19">
+        <v>0.13343618265141499</v>
+      </c>
+      <c r="H19">
+        <v>17</v>
+      </c>
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="J19" t="s">
+        <v>15</v>
+      </c>
+      <c r="K19">
+        <v>28</v>
+      </c>
+      <c r="L19">
+        <v>2.5599146772682899</v>
+      </c>
+      <c r="M19">
+        <v>0.120065569574871</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" t="s">
+        <v>14</v>
+      </c>
+      <c r="D20">
+        <v>24</v>
+      </c>
+      <c r="E20">
+        <v>2.66333333333333</v>
+      </c>
+      <c r="F20">
+        <v>0.111366000040013</v>
+      </c>
+      <c r="H20">
+        <v>18</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+      <c r="J20" t="s">
+        <v>15</v>
+      </c>
+      <c r="K20">
+        <v>28</v>
+      </c>
+      <c r="L20">
+        <v>2.6636470588235301</v>
+      </c>
+      <c r="M20">
+        <v>0.133915991005775</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>14</v>
+      </c>
+      <c r="D21">
+        <v>24</v>
+      </c>
+      <c r="E21">
+        <v>2.7275</v>
+      </c>
+      <c r="F21">
+        <v>7.19420172510742E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22">
+        <v>24</v>
+      </c>
+      <c r="E22">
+        <v>2.76981818181818</v>
+      </c>
+      <c r="F22">
+        <v>0.109572585600375</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23">
+        <v>24</v>
+      </c>
+      <c r="E23">
+        <v>2.6530810810810799</v>
+      </c>
+      <c r="F23">
+        <v>0.13486043082222099</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24">
+        <v>24</v>
+      </c>
+      <c r="E24">
+        <v>2.6127526881720402</v>
+      </c>
+      <c r="F24">
+        <v>0.11547676746522199</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>7</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25">
+        <v>24</v>
+      </c>
+      <c r="E25">
+        <v>2.6640000000000001</v>
+      </c>
+      <c r="F25">
+        <v>0.158349898882792</v>
+      </c>
+      <c r="H25" t="s">
+        <v>62</v>
+      </c>
+      <c r="I25" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26">
+        <v>24</v>
+      </c>
+      <c r="E26">
+        <v>2.69397202854082</v>
+      </c>
+      <c r="F26">
+        <v>0.132322714553187</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>20</v>
+      </c>
+      <c r="K26">
+        <v>2.7640934579439298</v>
+      </c>
+      <c r="L26">
+        <v>0.11347702405472999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27">
+        <v>24</v>
+      </c>
+      <c r="E27">
+        <v>2.7372195121951202</v>
+      </c>
+      <c r="F27">
+        <v>0.10472356759467299</v>
+      </c>
+      <c r="H27">
+        <v>2</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>20</v>
+      </c>
+      <c r="K27">
+        <v>2.8028668556070002</v>
+      </c>
+      <c r="L27">
+        <v>0.129023611415027</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28">
+        <v>24</v>
+      </c>
+      <c r="E28">
+        <v>2.8380526315789498</v>
+      </c>
+      <c r="F28">
+        <v>0.14147495800561299</v>
+      </c>
+      <c r="H28">
+        <v>3</v>
+      </c>
+      <c r="I28">
+        <v>3</v>
+      </c>
+      <c r="J28">
+        <v>20</v>
+      </c>
+      <c r="K28">
+        <v>2.9993307086614198</v>
+      </c>
+      <c r="L28">
+        <v>0.130238246590203</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29">
+        <v>24</v>
+      </c>
+      <c r="E29">
+        <v>2.7746825396825399</v>
+      </c>
+      <c r="F29">
+        <v>0.118603272733611</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
+      <c r="I29">
+        <v>1</v>
+      </c>
+      <c r="J29">
+        <v>24</v>
+      </c>
+      <c r="K29">
+        <v>2.6032336448598099</v>
+      </c>
+      <c r="L29">
+        <v>0.12832161105786499</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30">
+        <v>28</v>
+      </c>
+      <c r="E30">
+        <v>2.4836481481481498</v>
+      </c>
+      <c r="F30">
+        <v>0.114917059082645</v>
+      </c>
+      <c r="H30">
+        <v>5</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>24</v>
+      </c>
+      <c r="K30">
+        <v>2.6663726237855698</v>
+      </c>
+      <c r="L30">
+        <v>0.13848960162131499</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>14</v>
+      </c>
+      <c r="D31">
+        <v>28</v>
+      </c>
+      <c r="E31">
+        <v>2.5000749999999998</v>
+      </c>
+      <c r="F31">
+        <v>0.11460751344721801</v>
+      </c>
+      <c r="H31">
+        <v>6</v>
+      </c>
+      <c r="I31">
+        <v>3</v>
+      </c>
+      <c r="J31">
+        <v>24</v>
+      </c>
+      <c r="K31">
+        <v>2.77241525423729</v>
+      </c>
+      <c r="L31">
+        <v>0.114023713703277</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>28</v>
+      </c>
+      <c r="E32">
+        <v>2.4615238095238099</v>
+      </c>
+      <c r="F32">
+        <v>0.15224257565910401</v>
+      </c>
+      <c r="H32">
+        <v>7</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
+      </c>
+      <c r="J32">
+        <v>28</v>
+      </c>
+      <c r="K32">
+        <v>2.5362213815789501</v>
+      </c>
+      <c r="L32">
+        <v>0.12835951716538099</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33">
+        <v>28</v>
+      </c>
+      <c r="E33">
+        <v>2.4860619492749998</v>
+      </c>
+      <c r="F33">
+        <v>0.13198885663704199</v>
+      </c>
+      <c r="H33">
+        <v>8</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33">
+        <v>28</v>
+      </c>
+      <c r="K33">
+        <v>2.52731891870312</v>
+      </c>
+      <c r="L33">
+        <v>0.13303904790642701</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34">
+        <v>28</v>
+      </c>
+      <c r="E34">
+        <v>2.51565384615385</v>
+      </c>
+      <c r="F34">
+        <v>9.3416462064324607E-2</v>
+      </c>
+      <c r="H34">
+        <v>9</v>
+      </c>
+      <c r="I34">
+        <v>3</v>
+      </c>
+      <c r="J34">
+        <v>28</v>
+      </c>
+      <c r="K34">
+        <v>2.6465757575757598</v>
+      </c>
+      <c r="L34">
+        <v>0.12088063076415299</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D35">
+        <v>28</v>
+      </c>
+      <c r="E35">
+        <v>2.6339999999999999</v>
+      </c>
+      <c r="F35">
+        <v>8.3365327191691499E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>14</v>
+      </c>
+      <c r="D36">
+        <v>28</v>
+      </c>
+      <c r="E36">
+        <v>2.6284375</v>
+      </c>
+      <c r="F36">
+        <v>0.106593913991372</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37">
+        <v>28</v>
+      </c>
+      <c r="E37">
+        <v>2.57485526315789</v>
+      </c>
+      <c r="F37">
+        <v>0.12212078217321</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38">
+        <v>28</v>
+      </c>
+      <c r="E38">
+        <v>2.56887777777778</v>
+      </c>
+      <c r="F38">
+        <v>0.134717250947573</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39">
+        <v>28</v>
+      </c>
+      <c r="E39">
+        <v>2.5235205479452101</v>
+      </c>
+      <c r="F39">
+        <v>0.109301330375791</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40">
+        <v>28</v>
+      </c>
+      <c r="E40">
+        <v>2.5565134511999998</v>
+      </c>
+      <c r="F40">
+        <v>0.11337732709614</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41">
+        <v>28</v>
+      </c>
+      <c r="E41">
+        <v>2.5811162790697701</v>
+      </c>
+      <c r="F41">
+        <v>0.112235553594157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42">
+        <v>28</v>
+      </c>
+      <c r="E42">
+        <v>2.7027857142857101</v>
+      </c>
+      <c r="F42">
+        <v>0.12331708882228901</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43">
+        <v>28</v>
+      </c>
+      <c r="E43">
+        <v>2.6636470588235301</v>
+      </c>
+      <c r="F43">
+        <v>0.133915991005775</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated files for better stats
</commit_message>
<xml_diff>
--- a/lifehist/2017_10_21 Life history descriptive info.xlsx
+++ b/lifehist/2017_10_21 Life history descriptive info.xlsx
@@ -854,14 +854,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -872,10 +872,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -14854,46 +14854,46 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="39" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="39" t="s">
+      <c r="G2" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="K2" s="38" t="s">
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="K2" s="39" t="s">
         <v>66</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="L2" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="M2" s="39" t="s">
         <v>130</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="N2" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="39" t="s">
+      <c r="O2" s="37" t="s">
         <v>86</v>
       </c>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
+      <c r="P2" s="37"/>
+      <c r="Q2" s="37"/>
     </row>
     <row r="3" spans="3:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
       <c r="G3" s="14">
         <v>20</v>
       </c>
@@ -14903,10 +14903,10 @@
       <c r="I3" s="14">
         <v>28</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
       <c r="O3" s="14">
         <v>20</v>
       </c>
@@ -14918,7 +14918,7 @@
       </c>
     </row>
     <row r="4" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="38" t="s">
         <v>69</v>
       </c>
       <c r="D4" s="12" t="s">
@@ -14939,7 +14939,7 @@
       <c r="I4" s="12">
         <v>146</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="38" t="s">
         <v>69</v>
       </c>
       <c r="L4" s="12" t="s">
@@ -14969,7 +14969,7 @@
       <c r="X4" s="40"/>
     </row>
     <row r="5" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C5" s="37"/>
+      <c r="C5" s="38"/>
       <c r="D5" s="12" t="s">
         <v>82</v>
       </c>
@@ -14988,7 +14988,7 @@
       <c r="I5" s="12">
         <v>211</v>
       </c>
-      <c r="K5" s="37"/>
+      <c r="K5" s="38"/>
       <c r="L5" s="12" t="s">
         <v>126</v>
       </c>
@@ -15016,7 +15016,7 @@
       <c r="X5" s="2"/>
     </row>
     <row r="6" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C6" s="37"/>
+      <c r="C6" s="38"/>
       <c r="D6" s="12" t="s">
         <v>83</v>
       </c>
@@ -15035,7 +15035,7 @@
       <c r="I6" s="12">
         <v>224</v>
       </c>
-      <c r="K6" s="37"/>
+      <c r="K6" s="38"/>
       <c r="L6" s="12" t="s">
         <v>127</v>
       </c>
@@ -15063,7 +15063,7 @@
       <c r="X6" s="2"/>
     </row>
     <row r="7" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C7" s="37"/>
+      <c r="C7" s="38"/>
       <c r="D7" s="12" t="s">
         <v>83</v>
       </c>
@@ -15082,7 +15082,7 @@
       <c r="I7" s="12">
         <v>222</v>
       </c>
-      <c r="K7" s="37"/>
+      <c r="K7" s="38"/>
       <c r="L7" s="12" t="s">
         <v>127</v>
       </c>
@@ -15110,7 +15110,7 @@
       <c r="X7" s="2"/>
     </row>
     <row r="8" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="38" t="s">
         <v>70</v>
       </c>
       <c r="D8" s="12" t="s">
@@ -15131,7 +15131,7 @@
       <c r="I8" s="12">
         <v>120</v>
       </c>
-      <c r="K8" s="37" t="s">
+      <c r="K8" s="38" t="s">
         <v>70</v>
       </c>
       <c r="L8" s="12" t="s">
@@ -15161,7 +15161,7 @@
       <c r="X8" s="2"/>
     </row>
     <row r="9" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C9" s="37"/>
+      <c r="C9" s="38"/>
       <c r="D9" s="12" t="s">
         <v>84</v>
       </c>
@@ -15180,7 +15180,7 @@
       <c r="I9" s="12">
         <v>60</v>
       </c>
-      <c r="K9" s="37"/>
+      <c r="K9" s="38"/>
       <c r="L9" s="12" t="s">
         <v>128</v>
       </c>
@@ -15278,6 +15278,16 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="C8:C9"/>
@@ -15285,16 +15295,6 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -18072,7 +18072,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
@@ -21906,25 +21906,25 @@
       <c r="J3" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="L3" s="43" t="s">
+      <c r="L3" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="M3" s="44" t="s">
+      <c r="M3" s="43" t="s">
         <v>90</v>
       </c>
       <c r="N3" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="O3" s="43" t="s">
+      <c r="O3" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="P3" s="43" t="s">
+      <c r="P3" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="Q3" s="44" t="s">
+      <c r="Q3" s="43" t="s">
         <v>90</v>
       </c>
     </row>
@@ -21932,15 +21932,15 @@
       <c r="J4" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="43"/>
       <c r="N4" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="44"/>
+      <c r="O4" s="44"/>
+      <c r="P4" s="44"/>
+      <c r="Q4" s="43"/>
     </row>
     <row r="5" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J5" s="22">
@@ -22260,37 +22260,37 @@
       <c r="J18" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K18" s="43" t="s">
+      <c r="K18" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="L18" s="43" t="s">
+      <c r="L18" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="M18" s="44" t="s">
+      <c r="M18" s="43" t="s">
         <v>90</v>
       </c>
       <c r="N18" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="O18" s="43" t="s">
+      <c r="O18" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="P18" s="43" t="s">
+      <c r="P18" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="Q18" s="44" t="s">
+      <c r="Q18" s="43" t="s">
         <v>90</v>
       </c>
       <c r="R18" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="S18" s="43" t="s">
+      <c r="S18" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="T18" s="43" t="s">
+      <c r="T18" s="44" t="s">
         <v>102</v>
       </c>
-      <c r="U18" s="44" t="s">
+      <c r="U18" s="43" t="s">
         <v>90</v>
       </c>
     </row>
@@ -22298,21 +22298,21 @@
       <c r="J19" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="K19" s="43"/>
-      <c r="L19" s="43"/>
-      <c r="M19" s="44"/>
+      <c r="K19" s="44"/>
+      <c r="L19" s="44"/>
+      <c r="M19" s="43"/>
       <c r="N19" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="O19" s="43"/>
-      <c r="P19" s="43"/>
-      <c r="Q19" s="44"/>
+      <c r="O19" s="44"/>
+      <c r="P19" s="44"/>
+      <c r="Q19" s="43"/>
       <c r="R19" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="S19" s="43"/>
-      <c r="T19" s="43"/>
-      <c r="U19" s="44"/>
+      <c r="S19" s="44"/>
+      <c r="T19" s="44"/>
+      <c r="U19" s="43"/>
     </row>
     <row r="20" spans="10:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J20" s="22">
@@ -22514,11 +22514,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="M3:M4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="S18:S19"/>
     <mergeCell ref="T18:T19"/>
     <mergeCell ref="U18:U19"/>
     <mergeCell ref="J2:M2"/>
@@ -22534,6 +22529,11 @@
     <mergeCell ref="Q18:Q19"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
+    <mergeCell ref="M3:M4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="S18:S19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -24167,14 +24167,14 @@
         <v>33</v>
       </c>
       <c r="P14" s="16"/>
-      <c r="Q14" s="39" t="s">
+      <c r="Q14" s="37" t="s">
         <v>99</v>
       </c>
-      <c r="R14" s="39"/>
-      <c r="S14" s="39"/>
-      <c r="T14" s="39"/>
-      <c r="U14" s="39"/>
-      <c r="V14" s="39"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="37"/>
+      <c r="U14" s="37"/>
+      <c r="V14" s="37"/>
     </row>
     <row r="15" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" t="s">

</xml_diff>

<commit_message>
little life hist update?
</commit_message>
<xml_diff>
--- a/lifehist/2017_10_21 Life history descriptive info.xlsx
+++ b/lifehist/2017_10_21 Life history descriptive info.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmc04\Documents\GitHub\wingproj\lifehist\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\virgc\GitHub\wingproj\lifehist\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21765" windowHeight="10245" firstSheet="6" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21765" windowHeight="10245" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="First descriptive table" sheetId="2" r:id="rId1"/>
@@ -509,7 +509,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -854,14 +854,14 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -872,10 +872,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -14834,66 +14834,66 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:X12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:Q10"/>
+      <selection activeCell="C2" sqref="C2:I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="3" max="3" width="17.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="9" width="13.7109375" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.73046875" customWidth="1"/>
+    <col min="4" max="4" width="25.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.265625" customWidth="1"/>
+    <col min="7" max="9" width="13.73046875" customWidth="1"/>
+    <col min="11" max="11" width="15.59765625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
-    <col min="15" max="17" width="12.5703125" customWidth="1"/>
+    <col min="15" max="17" width="12.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="C2" s="39" t="s">
+    <row r="2" spans="3:24" ht="17.649999999999999" x14ac:dyDescent="0.5">
+      <c r="C2" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="39" t="s">
+      <c r="E2" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="37" t="s">
+      <c r="G2" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="K2" s="39" t="s">
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="K2" s="38" t="s">
         <v>66</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="L2" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="M2" s="39" t="s">
+      <c r="M2" s="38" t="s">
         <v>130</v>
       </c>
-      <c r="N2" s="39" t="s">
+      <c r="N2" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="O2" s="37" t="s">
+      <c r="O2" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="P2" s="37"/>
-      <c r="Q2" s="37"/>
-    </row>
-    <row r="3" spans="3:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+    </row>
+    <row r="3" spans="3:24" ht="30" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
       <c r="G3" s="14">
         <v>20</v>
       </c>
@@ -14903,10 +14903,10 @@
       <c r="I3" s="14">
         <v>28</v>
       </c>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
       <c r="O3" s="14">
         <v>20</v>
       </c>
@@ -14917,8 +14917,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="38" t="s">
+    <row r="4" spans="3:24" ht="15.75" x14ac:dyDescent="0.5">
+      <c r="C4" s="37" t="s">
         <v>69</v>
       </c>
       <c r="D4" s="12" t="s">
@@ -14939,7 +14939,7 @@
       <c r="I4" s="12">
         <v>146</v>
       </c>
-      <c r="K4" s="38" t="s">
+      <c r="K4" s="37" t="s">
         <v>69</v>
       </c>
       <c r="L4" s="12" t="s">
@@ -14968,8 +14968,8 @@
       <c r="W4" s="40"/>
       <c r="X4" s="40"/>
     </row>
-    <row r="5" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C5" s="38"/>
+    <row r="5" spans="3:24" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C5" s="37"/>
       <c r="D5" s="12" t="s">
         <v>82</v>
       </c>
@@ -14988,7 +14988,7 @@
       <c r="I5" s="12">
         <v>211</v>
       </c>
-      <c r="K5" s="38"/>
+      <c r="K5" s="37"/>
       <c r="L5" s="12" t="s">
         <v>126</v>
       </c>
@@ -15015,8 +15015,8 @@
       <c r="W5" s="2"/>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C6" s="38"/>
+    <row r="6" spans="3:24" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C6" s="37"/>
       <c r="D6" s="12" t="s">
         <v>83</v>
       </c>
@@ -15035,7 +15035,7 @@
       <c r="I6" s="12">
         <v>224</v>
       </c>
-      <c r="K6" s="38"/>
+      <c r="K6" s="37"/>
       <c r="L6" s="12" t="s">
         <v>127</v>
       </c>
@@ -15062,8 +15062,8 @@
       <c r="W6" s="2"/>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C7" s="38"/>
+    <row r="7" spans="3:24" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C7" s="37"/>
       <c r="D7" s="12" t="s">
         <v>83</v>
       </c>
@@ -15082,7 +15082,7 @@
       <c r="I7" s="12">
         <v>222</v>
       </c>
-      <c r="K7" s="38"/>
+      <c r="K7" s="37"/>
       <c r="L7" s="12" t="s">
         <v>127</v>
       </c>
@@ -15109,8 +15109,8 @@
       <c r="W7" s="2"/>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C8" s="38" t="s">
+    <row r="8" spans="3:24" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C8" s="37" t="s">
         <v>70</v>
       </c>
       <c r="D8" s="12" t="s">
@@ -15131,7 +15131,7 @@
       <c r="I8" s="12">
         <v>120</v>
       </c>
-      <c r="K8" s="38" t="s">
+      <c r="K8" s="37" t="s">
         <v>70</v>
       </c>
       <c r="L8" s="12" t="s">
@@ -15160,8 +15160,8 @@
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C9" s="38"/>
+    <row r="9" spans="3:24" ht="15.4" x14ac:dyDescent="0.45">
+      <c r="C9" s="37"/>
       <c r="D9" s="12" t="s">
         <v>84</v>
       </c>
@@ -15180,7 +15180,7 @@
       <c r="I9" s="12">
         <v>60</v>
       </c>
-      <c r="K9" s="38"/>
+      <c r="K9" s="37"/>
       <c r="L9" s="12" t="s">
         <v>128</v>
       </c>
@@ -15207,7 +15207,7 @@
       <c r="W9" s="2"/>
       <c r="X9" s="2"/>
     </row>
-    <row r="10" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:24" ht="15.4" x14ac:dyDescent="0.45">
       <c r="C10" s="15" t="s">
         <v>71</v>
       </c>
@@ -15258,7 +15258,7 @@
       <c r="W10" s="2"/>
       <c r="X10" s="2"/>
     </row>
-    <row r="11" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:24" x14ac:dyDescent="0.45">
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
@@ -15267,7 +15267,7 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
     </row>
-    <row r="12" spans="3:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:24" x14ac:dyDescent="0.45">
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
       <c r="T12" s="2"/>
@@ -15278,16 +15278,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="C8:C9"/>
@@ -15295,6 +15285,16 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15302,16 +15302,16 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -15349,7 +15349,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -15387,7 +15387,7 @@
         <v>4.6005837960550596E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -15425,7 +15425,7 @@
         <v>4.1535570255044297E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -15463,7 +15463,7 @@
         <v>3.9518225135399803E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -15501,7 +15501,7 @@
         <v>4.7552929659275198E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -15539,7 +15539,7 @@
         <v>4.0462210264209297E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -15577,7 +15577,7 @@
         <v>2.73285554260423E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -15615,7 +15615,7 @@
         <v>6.8273972839351799E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -15653,7 +15653,7 @@
         <v>6.5843564454429997E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -15691,7 +15691,7 @@
         <v>5.10891835107886E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -15729,7 +15729,7 @@
         <v>7.0225741124814098E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -15767,7 +15767,7 @@
         <v>6.3819392618997004E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -15805,7 +15805,7 @@
         <v>7.3733144125158901E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -15843,7 +15843,7 @@
         <v>6.5290419590436303E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -15881,7 +15881,7 @@
         <v>9.1305853944295499E-3</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -15919,7 +15919,7 @@
         <v>1.18533134121737E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -15957,7 +15957,7 @@
         <v>8.0392190290710305E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -15995,7 +15995,7 @@
         <v>8.7084247576947292E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -16033,7 +16033,7 @@
         <v>1.1014567720900001E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -16053,7 +16053,7 @@
         <v>4.5047558308657304E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -16073,7 +16073,7 @@
         <v>4.6696759011506904E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -16093,7 +16093,7 @@
         <v>5.10891835107886E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -16128,7 +16128,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -16163,7 +16163,7 @@
         <v>4.6776287990507696E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -16198,7 +16198,7 @@
         <v>4.1015580674548004E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -16233,7 +16233,7 @@
         <v>3.4146026061889498E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>26</v>
       </c>
@@ -16268,7 +16268,7 @@
         <v>6.9327539489770903E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -16303,7 +16303,7 @@
         <v>6.4847512790436298E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>28</v>
       </c>
@@ -16338,7 +16338,7 @@
         <v>6.5264471149675497E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>29</v>
       </c>
@@ -16373,7 +16373,7 @@
         <v>7.4315673317825398E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>30</v>
       </c>
@@ -16408,7 +16408,7 @@
         <v>8.9111960355018806E-3</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>31</v>
       </c>
@@ -16443,7 +16443,7 @@
         <v>1.1409147277194999E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>32</v>
       </c>
@@ -16463,7 +16463,7 @@
         <v>9.6188567039570995E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>33</v>
       </c>
@@ -16483,7 +16483,7 @@
         <v>7.9492467513650692E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>34</v>
       </c>
@@ -16503,7 +16503,7 @@
         <v>4.8562199439069103E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>35</v>
       </c>
@@ -16523,7 +16523,7 @@
         <v>1.18533134121737E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>36</v>
       </c>
@@ -16543,7 +16543,7 @@
         <v>7.7823316725343398E-3</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>37</v>
       </c>
@@ -16563,7 +16563,7 @@
         <v>7.2756437133648403E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>38</v>
       </c>
@@ -16583,7 +16583,7 @@
         <v>8.2045009122515607E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>39</v>
       </c>
@@ -16603,7 +16603,7 @@
         <v>8.73595623713775E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>40</v>
       </c>
@@ -16623,7 +16623,7 @@
         <v>8.4179066126182506E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>41</v>
       </c>
@@ -16643,7 +16643,7 @@
         <v>6.0615640516936704E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>42</v>
       </c>
@@ -16670,16 +16670,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="H40" sqref="H40:O48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -16717,7 +16717,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -16755,7 +16755,7 @@
         <v>5.8728236519264799E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -16793,7 +16793,7 @@
         <v>5.4273258985075099E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -16831,7 +16831,7 @@
         <v>5.3582642893852204E-3</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -16869,7 +16869,7 @@
         <v>6.0471072346911401E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -16907,7 +16907,7 @@
         <v>5.3386488843465297E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -16945,7 +16945,7 @@
         <v>3.96618502329368E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -16983,7 +16983,7 @@
         <v>8.3877821535513902E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -17021,7 +17021,7 @@
         <v>7.61443501850301E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -17059,7 +17059,7 @@
         <v>6.2067787176241299E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -17097,7 +17097,7 @@
         <v>8.7467924511133704E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -17135,7 +17135,7 @@
         <v>7.7773359381323702E-3</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -17173,7 +17173,7 @@
         <v>8.8922245532348995E-3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -17211,7 +17211,7 @@
         <v>8.2634341923764499E-3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -17249,7 +17249,7 @@
         <v>1.06938789877785E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -17287,7 +17287,7 @@
         <v>1.31407472371946E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -17325,7 +17325,7 @@
         <v>9.7218452412817999E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -17363,7 +17363,7 @@
         <v>1.02301661853802E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -17401,7 +17401,7 @@
         <v>1.27034328779662E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -17421,7 +17421,7 @@
         <v>5.70722474683654E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -17441,7 +17441,7 @@
         <v>5.7340877833706397E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -17461,7 +17461,7 @@
         <v>6.2067787176241299E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -17490,7 +17490,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -17525,7 +17525,7 @@
         <v>5.9603138914077498E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -17560,7 +17560,7 @@
         <v>5.3924055729636603E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -17595,7 +17595,7 @@
         <v>4.7395783739992503E-3</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>26</v>
       </c>
@@ -17630,7 +17630,7 @@
         <v>8.5896310528905898E-3</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -17665,7 +17665,7 @@
         <v>7.7021961504467199E-3</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>28</v>
       </c>
@@ -17700,7 +17700,7 @@
         <v>7.8762082602075699E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>29</v>
       </c>
@@ -17735,7 +17735,7 @@
         <v>9.1592622078111308E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>30</v>
       </c>
@@ -17770,7 +17770,7 @@
         <v>1.0459731682159201E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>31</v>
       </c>
@@ -17805,7 +17805,7 @@
         <v>1.2810825659831699E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>32</v>
       </c>
@@ -17825,7 +17825,7 @@
         <v>1.12949292304672E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>33</v>
       </c>
@@ -17845,7 +17845,7 @@
         <v>8.8862822357908301E-3</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>34</v>
       </c>
@@ -17865,7 +17865,7 @@
         <v>6.0182346264065802E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>35</v>
       </c>
@@ -17885,7 +17885,7 @@
         <v>1.31407472371946E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>36</v>
       </c>
@@ -17905,7 +17905,7 @@
         <v>1.0107172224713801E-2</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>37</v>
       </c>
@@ -17925,7 +17925,7 @@
         <v>7.7428733544034701E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>38</v>
       </c>
@@ -17945,7 +17945,7 @@
         <v>9.2802244627989295E-3</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>39</v>
       </c>
@@ -17968,7 +17968,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>40</v>
       </c>
@@ -17991,7 +17991,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>41</v>
       </c>
@@ -18014,7 +18014,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>42</v>
       </c>
@@ -18037,27 +18037,27 @@
         <v>141</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
       <c r="H44" s="36" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
       <c r="H45" s="36" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
       <c r="H46" s="36" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
       <c r="H47" s="36" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
       <c r="H48" s="36" t="s">
         <v>146</v>
       </c>
@@ -18069,16 +18069,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -18110,7 +18110,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -18148,7 +18148,7 @@
         <v>0.84052623285963801</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -18186,7 +18186,7 @@
         <v>0.98231379927013696</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -18224,7 +18224,7 @@
         <v>1.1795657215158899</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -18262,7 +18262,7 @@
         <v>1.2156264999303299</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -18300,7 +18300,7 @@
         <v>0.98733606238454896</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -18338,7 +18338,7 @@
         <v>1.03843199768925</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -18376,7 +18376,7 @@
         <v>0.65787424063262001</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -18414,7 +18414,7 @@
         <v>0.69860446088690598</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -18452,7 +18452,7 @@
         <v>0.77354439259702201</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -18490,7 +18490,7 @@
         <v>0.71654159369908299</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -18528,7 +18528,7 @@
         <v>0.77900152342211504</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -18566,7 +18566,7 @@
         <v>0.53261898546989805</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>13</v>
       </c>
@@ -18604,7 +18604,7 @@
         <v>0.41161835922658102</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>14</v>
       </c>
@@ -18642,7 +18642,7 @@
         <v>0.50608086578923805</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>15</v>
       </c>
@@ -18680,7 +18680,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>16</v>
       </c>
@@ -18718,7 +18718,7 @@
         <v>0.437097982963495</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>17</v>
       </c>
@@ -18756,7 +18756,7 @@
         <v>0.57961742756380996</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>18</v>
       </c>
@@ -18794,7 +18794,7 @@
         <v>0.63593377383645999</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>19</v>
       </c>
@@ -18814,7 +18814,7 @@
         <v>0.65611569473534803</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>20</v>
       </c>
@@ -18834,7 +18834,7 @@
         <v>0.51639777949432197</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>21</v>
       </c>
@@ -18854,7 +18854,7 @@
         <v>0.77354439259702201</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>22</v>
       </c>
@@ -18874,7 +18874,7 @@
         <v>0.68230086144930602</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>23</v>
       </c>
@@ -18903,7 +18903,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>24</v>
       </c>
@@ -18938,7 +18938,7 @@
         <v>1.06652727828992</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>25</v>
       </c>
@@ -18973,7 +18973,7 @@
         <v>0.99514463512134799</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>26</v>
       </c>
@@ -19008,7 +19008,7 @@
         <v>1.1991599126571999</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28">
         <v>27</v>
       </c>
@@ -19043,7 +19043,7 @@
         <v>0.71999855276818303</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>28</v>
       </c>
@@ -19078,7 +19078,7 @@
         <v>0.74462401912624299</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>29</v>
       </c>
@@ -19113,7 +19113,7 @@
         <v>0.65936289671281101</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>30</v>
       </c>
@@ -19148,7 +19148,7 @@
         <v>0.43375519782328498</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>31</v>
       </c>
@@ -19183,7 +19183,7 @@
         <v>0.55503875719815499</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>32</v>
       </c>
@@ -19218,7 +19218,7 @@
         <v>0.49619766344887301</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>33</v>
       </c>
@@ -19238,7 +19238,7 @@
         <v>0.33757978902788899</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A35">
         <v>34</v>
       </c>
@@ -19258,7 +19258,7 @@
         <v>0.42163702135578401</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A36">
         <v>35</v>
       </c>
@@ -19278,7 +19278,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A37">
         <v>36</v>
       </c>
@@ -19298,7 +19298,7 @@
         <v>0.32227263166891301</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>37</v>
       </c>
@@ -19318,7 +19318,7 @@
         <v>0.51304198621131203</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>38</v>
       </c>
@@ -19338,7 +19338,7 @@
         <v>0.58204117536868605</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>39</v>
       </c>
@@ -19358,7 +19358,7 @@
         <v>0.60247021749656904</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>40</v>
       </c>
@@ -19378,7 +19378,7 @@
         <v>0.56827694763887704</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>41</v>
       </c>
@@ -19398,7 +19398,7 @@
         <v>0.39223227027636798</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>42</v>
       </c>
@@ -19425,16 +19425,16 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:N92"/>
   <sheetViews>
     <sheetView topLeftCell="I48" workbookViewId="0">
       <selection activeCell="AF74" sqref="AF74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>21</v>
       </c>
@@ -19454,7 +19454,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B2">
         <v>1</v>
       </c>
@@ -19492,7 +19492,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="3" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B3">
         <v>2</v>
       </c>
@@ -19530,7 +19530,7 @@
         <v>0.11137784783772101</v>
       </c>
     </row>
-    <row r="4" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B4">
         <v>3</v>
       </c>
@@ -19568,7 +19568,7 @@
         <v>0.123948216129286</v>
       </c>
     </row>
-    <row r="5" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B5">
         <v>4</v>
       </c>
@@ -19606,7 +19606,7 @@
         <v>0.125327075931494</v>
       </c>
     </row>
-    <row r="6" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B6">
         <v>5</v>
       </c>
@@ -19644,7 +19644,7 @@
         <v>0.110758084532212</v>
       </c>
     </row>
-    <row r="7" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B7">
         <v>6</v>
       </c>
@@ -19682,7 +19682,7 @@
         <v>0.13056743316289399</v>
       </c>
     </row>
-    <row r="8" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B8">
         <v>7</v>
       </c>
@@ -19720,7 +19720,7 @@
         <v>0.13290690491023599</v>
       </c>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B9">
         <v>8</v>
       </c>
@@ -19758,7 +19758,7 @@
         <v>0.124895311394186</v>
       </c>
     </row>
-    <row r="10" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B10">
         <v>9</v>
       </c>
@@ -19796,7 +19796,7 @@
         <v>0.12098601546047601</v>
       </c>
     </row>
-    <row r="11" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B11">
         <v>10</v>
       </c>
@@ -19834,7 +19834,7 @@
         <v>0.109572585600375</v>
       </c>
     </row>
-    <row r="12" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B12">
         <v>11</v>
       </c>
@@ -19872,7 +19872,7 @@
         <v>0.125667069076184</v>
       </c>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B13">
         <v>12</v>
       </c>
@@ -19910,7 +19910,7 @@
         <v>0.14567084051402701</v>
       </c>
     </row>
-    <row r="14" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B14">
         <v>13</v>
       </c>
@@ -19948,7 +19948,7 @@
         <v>0.118603272733611</v>
       </c>
     </row>
-    <row r="15" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B15">
         <v>14</v>
       </c>
@@ -19986,7 +19986,7 @@
         <v>0.114591598010512</v>
       </c>
     </row>
-    <row r="16" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B16">
         <v>15</v>
       </c>
@@ -20024,7 +20024,7 @@
         <v>0.137612043011724</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B17">
         <v>16</v>
       </c>
@@ -20062,7 +20062,7 @@
         <v>0.106593913991372</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B18">
         <v>17</v>
       </c>
@@ -20100,7 +20100,7 @@
         <v>0.128752083250017</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B19">
         <v>18</v>
       </c>
@@ -20138,7 +20138,7 @@
         <v>0.120065569574871</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B20">
         <v>19</v>
       </c>
@@ -20176,7 +20176,7 @@
         <v>0.133915991005775</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B21">
         <v>20</v>
       </c>
@@ -20196,7 +20196,7 @@
         <v>7.19420172510742E-2</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B22">
         <v>21</v>
       </c>
@@ -20216,7 +20216,7 @@
         <v>0.109572585600375</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B23">
         <v>22</v>
       </c>
@@ -20236,7 +20236,7 @@
         <v>0.13486043082222099</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B24">
         <v>23</v>
       </c>
@@ -20256,7 +20256,7 @@
         <v>0.11547676746522199</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B25">
         <v>24</v>
       </c>
@@ -20285,7 +20285,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B26">
         <v>25</v>
       </c>
@@ -20320,7 +20320,7 @@
         <v>0.11347702405472999</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B27">
         <v>26</v>
       </c>
@@ -20355,7 +20355,7 @@
         <v>0.129023611415027</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B28">
         <v>27</v>
       </c>
@@ -20390,7 +20390,7 @@
         <v>0.130238246590203</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B29">
         <v>28</v>
       </c>
@@ -20425,7 +20425,7 @@
         <v>0.12832161105786499</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B30">
         <v>29</v>
       </c>
@@ -20460,7 +20460,7 @@
         <v>0.13848960162131499</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B31">
         <v>30</v>
       </c>
@@ -20495,7 +20495,7 @@
         <v>0.114023713703277</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.45">
       <c r="B32">
         <v>31</v>
       </c>
@@ -20530,7 +20530,7 @@
         <v>0.12835951716538099</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B33">
         <v>32</v>
       </c>
@@ -20565,7 +20565,7 @@
         <v>0.13303904790642701</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B34">
         <v>33</v>
       </c>
@@ -20600,7 +20600,7 @@
         <v>0.12088063076415299</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B35">
         <v>34</v>
       </c>
@@ -20620,7 +20620,7 @@
         <v>8.3365327191691499E-2</v>
       </c>
     </row>
-    <row r="36" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B36">
         <v>35</v>
       </c>
@@ -20640,7 +20640,7 @@
         <v>0.106593913991372</v>
       </c>
     </row>
-    <row r="37" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B37">
         <v>36</v>
       </c>
@@ -20660,7 +20660,7 @@
         <v>0.12212078217321</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B38">
         <v>37</v>
       </c>
@@ -20680,7 +20680,7 @@
         <v>0.134717250947573</v>
       </c>
     </row>
-    <row r="39" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B39">
         <v>38</v>
       </c>
@@ -20700,7 +20700,7 @@
         <v>0.109301330375791</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B40">
         <v>39</v>
       </c>
@@ -20720,7 +20720,7 @@
         <v>0.11337732709614</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B41">
         <v>40</v>
       </c>
@@ -20740,7 +20740,7 @@
         <v>0.112235553594157</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B42">
         <v>41</v>
       </c>
@@ -20760,7 +20760,7 @@
         <v>0.12331708882228901</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.45">
       <c r="B43">
         <v>42</v>
       </c>
@@ -20780,7 +20780,7 @@
         <v>0.133915991005775</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.45">
       <c r="H47" t="s">
         <v>148</v>
       </c>
@@ -20791,7 +20791,7 @@
         <v>1.108396E-2</v>
       </c>
     </row>
-    <row r="48" spans="2:13" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:13" x14ac:dyDescent="0.45">
       <c r="H48" t="s">
         <v>147</v>
       </c>
@@ -20802,7 +20802,7 @@
         <v>1.162321E-2</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="H49" t="s">
         <v>12</v>
       </c>
@@ -20813,7 +20813,7 @@
         <v>8.9508290000000004E-3</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B50" t="s">
         <v>21</v>
       </c>
@@ -20836,7 +20836,7 @@
         <v>3.8364950000000001E-3</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51">
         <f>ABS(B51)</f>
         <v>2.8639999999999999</v>
@@ -20860,7 +20860,7 @@
         <v>0.121703159310575</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52">
         <f t="shared" ref="A52:A92" si="0">ABS(B52)</f>
         <v>3.028</v>
@@ -20884,7 +20884,7 @@
         <v>0.104078280160915</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>8.7420000000000009</v>
@@ -20908,7 +20908,7 @@
         <v>0.12535685113065001</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>9.2230000000000008</v>
@@ -20932,7 +20932,7 @@
         <v>0.119848457692754</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>10.7</v>
@@ -20956,7 +20956,7 @@
         <v>0.120182951902467</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56">
         <f t="shared" si="0"/>
         <v>10.795999999999999</v>
@@ -20980,7 +20980,7 @@
         <v>0.13706042033909499</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57">
         <f t="shared" si="0"/>
         <v>22.611000000000001</v>
@@ -21004,7 +21004,7 @@
         <v>0.125327075931494</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58">
         <f t="shared" si="0"/>
         <v>2.8639999999999999</v>
@@ -21028,7 +21028,7 @@
         <v>0.11069182776141499</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59">
         <f t="shared" si="0"/>
         <v>3.028</v>
@@ -21052,7 +21052,7 @@
         <v>0.110239404645679</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60">
         <f t="shared" si="0"/>
         <v>8.7420000000000009</v>
@@ -21076,7 +21076,7 @@
         <v>0.13882151754261299</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61">
         <f t="shared" si="0"/>
         <v>9.2230000000000008</v>
@@ -21100,7 +21100,7 @@
         <v>0.114780209983717</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62">
         <f t="shared" si="0"/>
         <v>10.7</v>
@@ -21124,7 +21124,7 @@
         <v>0.13301658761576901</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63">
         <f t="shared" si="0"/>
         <v>10.795999999999999</v>
@@ -21148,7 +21148,7 @@
         <v>0.14530917524456699</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64">
         <f t="shared" si="0"/>
         <v>22.611000000000001</v>
@@ -21172,7 +21172,7 @@
         <v>0.13290690491023599</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65">
         <f t="shared" si="0"/>
         <v>2.8639999999999999</v>
@@ -21196,7 +21196,7 @@
         <v>0.121065935400036</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66">
         <f t="shared" si="0"/>
         <v>3.028</v>
@@ -21220,7 +21220,7 @@
         <v>0.122882783655117</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67">
         <f t="shared" si="0"/>
         <v>8.7420000000000009</v>
@@ -21244,7 +21244,7 @@
         <v>0.10878021648406599</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68">
         <f t="shared" si="0"/>
         <v>9.2230000000000008</v>
@@ -21268,7 +21268,7 @@
         <v>0.13343618265141499</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69">
         <f t="shared" si="0"/>
         <v>10.7</v>
@@ -21292,7 +21292,7 @@
         <v>0.111366000040013</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70">
         <f t="shared" si="0"/>
         <v>10.795999999999999</v>
@@ -21316,7 +21316,7 @@
         <v>7.19420172510742E-2</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71">
         <f t="shared" si="0"/>
         <v>22.611000000000001</v>
@@ -21340,7 +21340,7 @@
         <v>0.109572585600375</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72">
         <f t="shared" si="0"/>
         <v>2.8639999999999999</v>
@@ -21364,7 +21364,7 @@
         <v>0.13486043082222099</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73">
         <f t="shared" si="0"/>
         <v>3.028</v>
@@ -21388,7 +21388,7 @@
         <v>0.11547676746522199</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74">
         <f t="shared" si="0"/>
         <v>8.7420000000000009</v>
@@ -21412,7 +21412,7 @@
         <v>0.158349898882792</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75">
         <f t="shared" si="0"/>
         <v>9.2230000000000008</v>
@@ -21436,7 +21436,7 @@
         <v>0.132322714553187</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A76">
         <f t="shared" si="0"/>
         <v>10.7</v>
@@ -21460,7 +21460,7 @@
         <v>0.10472356759467299</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A77">
         <f t="shared" si="0"/>
         <v>10.795999999999999</v>
@@ -21484,7 +21484,7 @@
         <v>0.14147495800561299</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A78">
         <f t="shared" si="0"/>
         <v>22.611000000000001</v>
@@ -21508,7 +21508,7 @@
         <v>0.118603272733611</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A79">
         <f t="shared" si="0"/>
         <v>2.8639999999999999</v>
@@ -21532,7 +21532,7 @@
         <v>0.114917059082645</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A80">
         <f t="shared" si="0"/>
         <v>3.028</v>
@@ -21556,7 +21556,7 @@
         <v>0.11460751344721801</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A81">
         <f t="shared" si="0"/>
         <v>8.7420000000000009</v>
@@ -21580,7 +21580,7 @@
         <v>0.15224257565910401</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A82">
         <f t="shared" si="0"/>
         <v>9.2230000000000008</v>
@@ -21604,7 +21604,7 @@
         <v>0.13198885663704199</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A83">
         <f t="shared" si="0"/>
         <v>10.7</v>
@@ -21628,7 +21628,7 @@
         <v>9.3416462064324607E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A84">
         <f t="shared" si="0"/>
         <v>10.795999999999999</v>
@@ -21652,7 +21652,7 @@
         <v>8.3365327191691499E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A85">
         <f t="shared" si="0"/>
         <v>22.611000000000001</v>
@@ -21676,7 +21676,7 @@
         <v>0.106593913991372</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A86">
         <f t="shared" si="0"/>
         <v>2.8639999999999999</v>
@@ -21700,7 +21700,7 @@
         <v>0.12212078217321</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A87">
         <f t="shared" si="0"/>
         <v>3.028</v>
@@ -21724,7 +21724,7 @@
         <v>0.134717250947573</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A88">
         <f t="shared" si="0"/>
         <v>8.7420000000000009</v>
@@ -21748,7 +21748,7 @@
         <v>0.109301330375791</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A89">
         <f t="shared" si="0"/>
         <v>9.2230000000000008</v>
@@ -21772,7 +21772,7 @@
         <v>0.11337732709614</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A90">
         <f t="shared" si="0"/>
         <v>10.7</v>
@@ -21796,7 +21796,7 @@
         <v>0.112235553594157</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A91">
         <f t="shared" si="0"/>
         <v>10.795999999999999</v>
@@ -21820,7 +21820,7 @@
         <v>0.12331708882228901</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A92">
         <f t="shared" si="0"/>
         <v>22.611000000000001</v>
@@ -21851,32 +21851,32 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="C1:V25"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J17" sqref="J17:U25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.59765625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.3984375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="24" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.3984375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="16" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.3984375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="24" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="22.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15.73046875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="2" spans="3:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="C2" t="s">
         <v>87</v>
       </c>
@@ -21893,7 +21893,7 @@
       <c r="P2" s="46"/>
       <c r="Q2" s="47"/>
     </row>
-    <row r="3" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="C3" t="s">
         <v>88</v>
       </c>
@@ -21906,43 +21906,43 @@
       <c r="J3" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K3" s="44" t="s">
+      <c r="K3" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="L3" s="44" t="s">
+      <c r="L3" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="M3" s="43" t="s">
+      <c r="M3" s="44" t="s">
         <v>90</v>
       </c>
       <c r="N3" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="O3" s="44" t="s">
+      <c r="O3" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="P3" s="44" t="s">
+      <c r="P3" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="Q3" s="43" t="s">
+      <c r="Q3" s="44" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="4" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="J4" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="K4" s="44"/>
-      <c r="L4" s="44"/>
-      <c r="M4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="44"/>
       <c r="N4" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="O4" s="44"/>
-      <c r="P4" s="44"/>
-      <c r="Q4" s="43"/>
-    </row>
-    <row r="5" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="44"/>
+    </row>
+    <row r="5" spans="3:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="J5" s="22">
         <v>1</v>
       </c>
@@ -21966,7 +21966,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="D6" t="s">
         <v>100</v>
       </c>
@@ -22022,7 +22022,7 @@
         <v>0.32119999999999999</v>
       </c>
     </row>
-    <row r="7" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
         <v>101</v>
       </c>
@@ -22081,7 +22081,7 @@
         <v>6.7800000000000013E-2</v>
       </c>
     </row>
-    <row r="8" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="F8">
         <v>0.15279999999999999</v>
       </c>
@@ -22123,7 +22123,7 @@
         <v>4.7615999999999996</v>
       </c>
     </row>
-    <row r="9" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="F9">
         <v>4.7416999999999998</v>
       </c>
@@ -22169,7 +22169,7 @@
         <v>13.2645</v>
       </c>
     </row>
-    <row r="10" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="F10">
         <v>13.553599999999999</v>
       </c>
@@ -22209,7 +22209,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="11" spans="3:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="J11" s="26">
         <v>28</v>
       </c>
@@ -22235,8 +22235,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="17" spans="10:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:22" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
+    <row r="17" spans="10:21" ht="15.4" x14ac:dyDescent="0.45">
       <c r="J17" s="45" t="s">
         <v>96</v>
       </c>
@@ -22256,65 +22256,65 @@
       <c r="T17" s="46"/>
       <c r="U17" s="47"/>
     </row>
-    <row r="18" spans="10:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="10:21" ht="15.4" x14ac:dyDescent="0.45">
       <c r="J18" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K18" s="44" t="s">
+      <c r="K18" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="L18" s="44" t="s">
+      <c r="L18" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="M18" s="43" t="s">
+      <c r="M18" s="44" t="s">
         <v>90</v>
       </c>
       <c r="N18" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="O18" s="44" t="s">
+      <c r="O18" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="P18" s="44" t="s">
+      <c r="P18" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="Q18" s="43" t="s">
+      <c r="Q18" s="44" t="s">
         <v>90</v>
       </c>
       <c r="R18" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="S18" s="44" t="s">
+      <c r="S18" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="T18" s="44" t="s">
+      <c r="T18" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="U18" s="43" t="s">
+      <c r="U18" s="44" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="19" spans="10:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="10:21" ht="15.4" x14ac:dyDescent="0.45">
       <c r="J19" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="K19" s="44"/>
-      <c r="L19" s="44"/>
-      <c r="M19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="44"/>
       <c r="N19" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="O19" s="44"/>
-      <c r="P19" s="44"/>
-      <c r="Q19" s="43"/>
+      <c r="O19" s="43"/>
+      <c r="P19" s="43"/>
+      <c r="Q19" s="44"/>
       <c r="R19" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="S19" s="44"/>
-      <c r="T19" s="44"/>
-      <c r="U19" s="43"/>
-    </row>
-    <row r="20" spans="10:21" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="S19" s="43"/>
+      <c r="T19" s="43"/>
+      <c r="U19" s="44"/>
+    </row>
+    <row r="20" spans="10:21" ht="15.4" x14ac:dyDescent="0.45">
       <c r="J20" s="22">
         <v>1</v>
       </c>
@@ -22340,7 +22340,7 @@
       </c>
       <c r="U20" s="23"/>
     </row>
-    <row r="21" spans="10:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="10:21" ht="15.4" x14ac:dyDescent="0.45">
       <c r="J21" s="22">
         <v>2</v>
       </c>
@@ -22378,7 +22378,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="10:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="10:21" ht="15.4" x14ac:dyDescent="0.45">
       <c r="J22" s="22">
         <v>3</v>
       </c>
@@ -22416,7 +22416,7 @@
         <v>3.8999999999999998E-14</v>
       </c>
     </row>
-    <row r="23" spans="10:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="10:21" ht="15.4" x14ac:dyDescent="0.45">
       <c r="J23" s="20" t="s">
         <v>59</v>
       </c>
@@ -22436,7 +22436,7 @@
       <c r="T23" s="11"/>
       <c r="U23" s="23"/>
     </row>
-    <row r="24" spans="10:21" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="10:21" ht="15.4" x14ac:dyDescent="0.45">
       <c r="J24" s="22" t="s">
         <v>91</v>
       </c>
@@ -22474,7 +22474,7 @@
         <v>7.5E-10</v>
       </c>
     </row>
-    <row r="25" spans="10:21" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="10:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.5">
       <c r="J25" s="26" t="s">
         <v>95</v>
       </c>
@@ -22514,6 +22514,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="S18:S19"/>
     <mergeCell ref="T18:T19"/>
     <mergeCell ref="U18:U19"/>
     <mergeCell ref="J2:M2"/>
@@ -22530,10 +22534,6 @@
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="M3:M4"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="S18:S19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -22541,26 +22541,26 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H25" activeCellId="1" sqref="D25:D45 H25:H45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -22574,7 +22574,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -22585,7 +22585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -22596,7 +22596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -22607,7 +22607,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -22618,7 +22618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -22629,7 +22629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -22640,7 +22640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -22651,7 +22651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -22662,7 +22662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -22673,7 +22673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -22684,7 +22684,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -22695,7 +22695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -22706,7 +22706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -22717,7 +22717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -22728,7 +22728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -22739,7 +22739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -22750,7 +22750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -22761,7 +22761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -22773,7 +22773,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -22784,7 +22784,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -22795,7 +22795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -22809,7 +22809,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>4</v>
       </c>
@@ -22845,7 +22845,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -22881,7 +22881,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -22917,7 +22917,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -22953,7 +22953,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -22989,7 +22989,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -23025,7 +23025,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -23061,7 +23061,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>4</v>
       </c>
@@ -23097,7 +23097,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>6</v>
       </c>
@@ -23133,7 +23133,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>7</v>
       </c>
@@ -23169,7 +23169,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>8</v>
       </c>
@@ -23205,7 +23205,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -23241,7 +23241,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -23277,7 +23277,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>11</v>
       </c>
@@ -23313,7 +23313,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>4</v>
       </c>
@@ -23349,7 +23349,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>6</v>
       </c>
@@ -23385,7 +23385,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>7</v>
       </c>
@@ -23421,7 +23421,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -23457,7 +23457,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -23493,7 +23493,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -23529,7 +23529,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -23571,26 +23571,26 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -23601,7 +23601,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -23612,7 +23612,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -23623,7 +23623,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -23634,7 +23634,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -23645,7 +23645,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -23656,7 +23656,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -23667,7 +23667,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -23678,7 +23678,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -23689,7 +23689,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>6</v>
       </c>
@@ -23700,7 +23700,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -23711,7 +23711,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -23722,7 +23722,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>9</v>
       </c>
@@ -23733,7 +23733,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -23744,7 +23744,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>11</v>
       </c>
@@ -23755,7 +23755,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -23766,7 +23766,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -23777,7 +23777,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -23788,7 +23788,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -23799,7 +23799,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -23810,7 +23810,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -23821,7 +23821,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -23838,16 +23838,16 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A6:V50"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="P14" sqref="P14:V23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:22" x14ac:dyDescent="0.45">
       <c r="G6" s="2"/>
       <c r="H6" s="40" t="s">
         <v>5</v>
@@ -23862,7 +23862,7 @@
       </c>
       <c r="M6" s="40"/>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:22" x14ac:dyDescent="0.45">
       <c r="D7" t="s">
         <v>25</v>
       </c>
@@ -23894,7 +23894,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -23933,7 +23933,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B9" t="s">
         <v>6</v>
       </c>
@@ -23972,7 +23972,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
         <v>7</v>
       </c>
@@ -24011,7 +24011,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -24050,7 +24050,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -24089,7 +24089,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:22" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
         <v>10</v>
       </c>
@@ -24128,7 +24128,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="2:22" ht="18" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:22" ht="17.649999999999999" x14ac:dyDescent="0.5">
       <c r="B14" t="s">
         <v>11</v>
       </c>
@@ -24167,16 +24167,16 @@
         <v>33</v>
       </c>
       <c r="P14" s="16"/>
-      <c r="Q14" s="37" t="s">
+      <c r="Q14" s="39" t="s">
         <v>99</v>
       </c>
-      <c r="R14" s="37"/>
-      <c r="S14" s="37"/>
-      <c r="T14" s="37"/>
-      <c r="U14" s="37"/>
-      <c r="V14" s="37"/>
-    </row>
-    <row r="15" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="R14" s="39"/>
+      <c r="S14" s="39"/>
+      <c r="T14" s="39"/>
+      <c r="U14" s="39"/>
+      <c r="V14" s="39"/>
+    </row>
+    <row r="15" spans="2:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
         <v>4</v>
       </c>
@@ -24207,7 +24207,7 @@
       </c>
       <c r="V15" s="42"/>
     </row>
-    <row r="16" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
         <v>6</v>
       </c>
@@ -24259,7 +24259,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>7</v>
       </c>
@@ -24317,7 +24317,7 @@
         <v>0.58461538461538465</v>
       </c>
     </row>
-    <row r="18" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>8</v>
       </c>
@@ -24378,7 +24378,7 @@
         <v>0.52513966480446927</v>
       </c>
     </row>
-    <row r="19" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>9</v>
       </c>
@@ -24439,7 +24439,7 @@
         <v>0.53900709219858156</v>
       </c>
     </row>
-    <row r="20" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>10</v>
       </c>
@@ -24500,7 +24500,7 @@
         <v>0.48749999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>11</v>
       </c>
@@ -24561,7 +24561,7 @@
         <v>0.61971830985915488</v>
       </c>
     </row>
-    <row r="22" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
         <v>4</v>
       </c>
@@ -24622,7 +24622,7 @@
         <v>0.58333333333333337</v>
       </c>
     </row>
-    <row r="23" spans="1:22" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" ht="15.4" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
         <v>6</v>
       </c>
@@ -24683,7 +24683,7 @@
         <v>0.51515151515151514</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
         <v>7</v>
       </c>
@@ -24717,7 +24717,7 @@
       </c>
       <c r="K24" s="5"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
         <v>8</v>
       </c>
@@ -24735,7 +24735,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>9</v>
       </c>
@@ -24753,7 +24753,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B27" t="s">
         <v>10</v>
       </c>
@@ -24771,7 +24771,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B28" t="s">
         <v>11</v>
       </c>
@@ -24789,7 +24789,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
         <v>14</v>
       </c>
@@ -24801,7 +24801,7 @@
         <v>2652</v>
       </c>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>5</v>
       </c>
@@ -24812,7 +24812,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>5</v>
       </c>
@@ -24823,7 +24823,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>5</v>
       </c>
@@ -24834,7 +24834,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>5</v>
       </c>
@@ -24845,7 +24845,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>5</v>
       </c>
@@ -24856,7 +24856,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>5</v>
       </c>
@@ -24867,7 +24867,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>5</v>
       </c>
@@ -24878,7 +24878,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>12</v>
       </c>
@@ -24889,7 +24889,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>12</v>
       </c>
@@ -24900,7 +24900,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>12</v>
       </c>
@@ -24911,7 +24911,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>12</v>
       </c>
@@ -24922,7 +24922,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>12</v>
       </c>
@@ -24933,7 +24933,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>12</v>
       </c>
@@ -24944,7 +24944,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>12</v>
       </c>
@@ -24955,7 +24955,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>13</v>
       </c>
@@ -24966,7 +24966,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>13</v>
       </c>
@@ -24977,7 +24977,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>13</v>
       </c>
@@ -24988,7 +24988,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>13</v>
       </c>
@@ -24999,7 +24999,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>13</v>
       </c>
@@ -25010,7 +25010,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>13</v>
       </c>
@@ -25021,7 +25021,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>13</v>
       </c>
@@ -25048,19 +25048,19 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -25083,7 +25083,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -25107,7 +25107,7 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -25127,7 +25127,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -25144,7 +25144,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -25161,7 +25161,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -25178,7 +25178,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -25195,7 +25195,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -25212,7 +25212,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -25229,7 +25229,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -25246,7 +25246,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -25263,7 +25263,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -25280,7 +25280,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -25297,7 +25297,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -25314,7 +25314,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -25331,7 +25331,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -25348,7 +25348,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -25365,7 +25365,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -25382,7 +25382,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -25399,7 +25399,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -25416,7 +25416,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -25433,7 +25433,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -25456,16 +25456,16 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -25479,7 +25479,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -25493,7 +25493,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -25507,7 +25507,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -25521,7 +25521,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -25535,7 +25535,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -25549,7 +25549,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -25563,7 +25563,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -25577,7 +25577,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -25591,7 +25591,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -25605,7 +25605,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -25619,7 +25619,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -25633,7 +25633,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -25647,7 +25647,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -25661,7 +25661,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -25675,7 +25675,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -25689,7 +25689,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -25703,7 +25703,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -25717,7 +25717,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -25731,7 +25731,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -25745,7 +25745,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -25759,7 +25759,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -25773,7 +25773,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -25787,7 +25787,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -25801,7 +25801,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -25815,7 +25815,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -25829,7 +25829,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -25843,7 +25843,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -25857,7 +25857,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -25871,7 +25871,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -25885,7 +25885,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -25899,7 +25899,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -25913,7 +25913,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -25927,7 +25927,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -25941,7 +25941,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -25955,7 +25955,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -25969,7 +25969,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -25983,7 +25983,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -25997,7 +25997,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -26011,7 +26011,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -26025,7 +26025,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -26039,7 +26039,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -26053,7 +26053,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -26073,153 +26073,153 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A2:A29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" s="7"/>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" s="8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A7" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A8" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A9" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A11" s="8"/>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A12" s="9" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A13" s="8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A14" s="7"/>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A16" s="8" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A18" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A19" s="8" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A20" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A21" s="8"/>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A22" s="9" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A26" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A27" s="7"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A28" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A29" s="8" t="s">
         <v>57</v>
       </c>
@@ -26230,16 +26230,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="AE23" sqref="AE23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -26286,7 +26286,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -26330,7 +26330,7 @@
         <v>2.16419990302707</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -26374,7 +26374,7 @@
         <v>2.2750455815333899</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -26418,7 +26418,7 @@
         <v>1.9486495382806699</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -26462,7 +26462,7 @@
         <v>2.1199653000846999</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -26506,7 +26506,7 @@
         <v>2.35153542935292</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -26550,7 +26550,7 @@
         <v>2.9918303680270601</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -26594,7 +26594,7 @@
         <v>1.8176916087570401</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -26638,7 +26638,7 @@
         <v>2.4435685896620698</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -26682,7 +26682,7 @@
         <v>3.7071076405768899</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -26699,7 +26699,7 @@
         <v>1.9970116231104</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -26716,7 +26716,7 @@
         <v>2.2077211009150899</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -26733,7 +26733,7 @@
         <v>2.60984402722432</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -26750,7 +26750,7 @@
         <v>2.0232168923292901</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -26767,7 +26767,7 @@
         <v>1.9486495382806699</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -26784,7 +26784,7 @@
         <v>2.1152566692820902</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -26801,7 +26801,7 @@
         <v>1.9855417995156299</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -26818,7 +26818,7 @@
         <v>1.9677870788774801</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -26835,7 +26835,7 @@
         <v>2.3984415627287201</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>9</v>
       </c>
@@ -26852,7 +26852,7 @@
         <v>2.0677547620783199</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -26869,7 +26869,7 @@
         <v>2.0071301473924001</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>11</v>
       </c>
@@ -26886,7 +26886,7 @@
         <v>2.3244100768826899</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -26903,7 +26903,7 @@
         <v>2.2676399939565202</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>6</v>
       </c>
@@ -26920,7 +26920,7 @@
         <v>1.98398874497972</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -26937,7 +26937,7 @@
         <v>2.3455578412964599</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -26954,7 +26954,7 @@
         <v>2.3749934861817898</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -26971,7 +26971,7 @@
         <v>1.8751153526716799</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -26988,7 +26988,7 @@
         <v>1.8027756377319899</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>11</v>
       </c>
@@ -27005,7 +27005,7 @@
         <v>2.9918303680270601</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>4</v>
       </c>
@@ -27022,7 +27022,7 @@
         <v>1.6682382527458499</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>6</v>
       </c>
@@ -27039,7 +27039,7 @@
         <v>1.41342106381696</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>7</v>
       </c>
@@ -27068,7 +27068,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>8</v>
       </c>
@@ -27097,7 +27097,7 @@
         <v>2.1129840764025301</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -27126,7 +27126,7 @@
         <v>2.3521321816515899</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -27155,7 +27155,7 @@
         <v>2.5094540235126899</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>11</v>
       </c>
@@ -27184,7 +27184,7 @@
         <v>2.1138281562827101</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>4</v>
       </c>
@@ -27213,7 +27213,7 @@
         <v>2.4028131475510301</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>6</v>
       </c>
@@ -27242,7 +27242,7 @@
         <v>2.7329006266235401</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>7</v>
       </c>
@@ -27271,7 +27271,7 @@
         <v>1.70231904640529</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -27300,7 +27300,7 @@
         <v>2.5308226510641201</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -27329,7 +27329,7 @@
         <v>3.5172733930151199</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -27346,7 +27346,7 @@
         <v>2.1737697038266801</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Some life history changes
perfected some ggplot
</commit_message>
<xml_diff>
--- a/lifehist/2017_10_21 Life history descriptive info.xlsx
+++ b/lifehist/2017_10_21 Life history descriptive info.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21765" windowHeight="10245" firstSheet="6" activeTab="13"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="21765" windowHeight="10245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="First descriptive table" sheetId="2" r:id="rId1"/>
@@ -509,7 +509,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -867,14 +867,20 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -891,6 +897,18 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -902,24 +920,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -14865,11 +14865,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C2:X12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:Q10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14885,16 +14885,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:24" ht="18" x14ac:dyDescent="0.25">
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="38" t="s">
+      <c r="D2" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="38" t="s">
+      <c r="E2" s="41" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="41" t="s">
         <v>72</v>
       </c>
       <c r="G2" s="39" t="s">
@@ -14902,16 +14902,16 @@
       </c>
       <c r="H2" s="39"/>
       <c r="I2" s="39"/>
-      <c r="K2" s="38" t="s">
+      <c r="K2" s="41" t="s">
         <v>66</v>
       </c>
-      <c r="L2" s="38" t="s">
+      <c r="L2" s="41" t="s">
         <v>125</v>
       </c>
-      <c r="M2" s="38" t="s">
+      <c r="M2" s="41" t="s">
         <v>130</v>
       </c>
-      <c r="N2" s="38" t="s">
+      <c r="N2" s="41" t="s">
         <v>72</v>
       </c>
       <c r="O2" s="39" t="s">
@@ -14921,10 +14921,10 @@
       <c r="Q2" s="39"/>
     </row>
     <row r="3" spans="3:24" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="38"/>
-      <c r="D3" s="38"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
       <c r="G3" s="14">
         <v>20</v>
       </c>
@@ -14934,10 +14934,10 @@
       <c r="I3" s="14">
         <v>28</v>
       </c>
-      <c r="K3" s="38"/>
-      <c r="L3" s="38"/>
-      <c r="M3" s="38"/>
-      <c r="N3" s="38"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="41"/>
+      <c r="N3" s="41"/>
       <c r="O3" s="14">
         <v>20</v>
       </c>
@@ -14949,7 +14949,7 @@
       </c>
     </row>
     <row r="4" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="40" t="s">
         <v>69</v>
       </c>
       <c r="D4" s="12" t="s">
@@ -14970,7 +14970,7 @@
       <c r="I4" s="12">
         <v>146</v>
       </c>
-      <c r="K4" s="37" t="s">
+      <c r="K4" s="40" t="s">
         <v>69</v>
       </c>
       <c r="L4" s="12" t="s">
@@ -14992,15 +14992,15 @@
         <v>146</v>
       </c>
       <c r="R4" s="2"/>
-      <c r="S4" s="40"/>
-      <c r="T4" s="40"/>
-      <c r="U4" s="40"/>
-      <c r="V4" s="40"/>
-      <c r="W4" s="40"/>
-      <c r="X4" s="40"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="42"/>
+      <c r="V4" s="42"/>
+      <c r="W4" s="42"/>
+      <c r="X4" s="42"/>
     </row>
     <row r="5" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C5" s="37"/>
+      <c r="C5" s="40"/>
       <c r="D5" s="12" t="s">
         <v>82</v>
       </c>
@@ -15019,7 +15019,7 @@
       <c r="I5" s="12">
         <v>211</v>
       </c>
-      <c r="K5" s="37"/>
+      <c r="K5" s="40"/>
       <c r="L5" s="12" t="s">
         <v>126</v>
       </c>
@@ -15047,7 +15047,7 @@
       <c r="X5" s="2"/>
     </row>
     <row r="6" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C6" s="37"/>
+      <c r="C6" s="40"/>
       <c r="D6" s="12" t="s">
         <v>83</v>
       </c>
@@ -15066,7 +15066,7 @@
       <c r="I6" s="12">
         <v>224</v>
       </c>
-      <c r="K6" s="37"/>
+      <c r="K6" s="40"/>
       <c r="L6" s="12" t="s">
         <v>127</v>
       </c>
@@ -15094,7 +15094,7 @@
       <c r="X6" s="2"/>
     </row>
     <row r="7" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C7" s="37"/>
+      <c r="C7" s="40"/>
       <c r="D7" s="12" t="s">
         <v>83</v>
       </c>
@@ -15113,7 +15113,7 @@
       <c r="I7" s="12">
         <v>222</v>
       </c>
-      <c r="K7" s="37"/>
+      <c r="K7" s="40"/>
       <c r="L7" s="12" t="s">
         <v>127</v>
       </c>
@@ -15141,7 +15141,7 @@
       <c r="X7" s="2"/>
     </row>
     <row r="8" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C8" s="37" t="s">
+      <c r="C8" s="40" t="s">
         <v>70</v>
       </c>
       <c r="D8" s="12" t="s">
@@ -15162,7 +15162,7 @@
       <c r="I8" s="12">
         <v>120</v>
       </c>
-      <c r="K8" s="37" t="s">
+      <c r="K8" s="40" t="s">
         <v>70</v>
       </c>
       <c r="L8" s="12" t="s">
@@ -15192,7 +15192,7 @@
       <c r="X8" s="2"/>
     </row>
     <row r="9" spans="3:24" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C9" s="37"/>
+      <c r="C9" s="40"/>
       <c r="D9" s="12" t="s">
         <v>84</v>
       </c>
@@ -15211,7 +15211,7 @@
       <c r="I9" s="12">
         <v>60</v>
       </c>
-      <c r="K9" s="37"/>
+      <c r="K9" s="40"/>
       <c r="L9" s="12" t="s">
         <v>128</v>
       </c>
@@ -15309,6 +15309,16 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="L2:L3"/>
+    <mergeCell ref="M2:M3"/>
+    <mergeCell ref="N2:N3"/>
+    <mergeCell ref="O2:Q2"/>
+    <mergeCell ref="K4:K7"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
     <mergeCell ref="G2:I2"/>
     <mergeCell ref="C4:C7"/>
     <mergeCell ref="C8:C9"/>
@@ -15316,16 +15326,6 @@
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="F2:F3"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="K4:K7"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="L2:L3"/>
-    <mergeCell ref="M2:M3"/>
-    <mergeCell ref="N2:N3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -15333,7 +15333,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView topLeftCell="E1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
@@ -16701,7 +16701,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:M48"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
@@ -18100,7 +18100,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
     <sheetView topLeftCell="A22" workbookViewId="0">
@@ -19456,7 +19456,7 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:N92"/>
   <sheetViews>
     <sheetView topLeftCell="I48" workbookViewId="0">
@@ -21882,10 +21882,10 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="C1:V25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="J17" sqref="J17:U25"/>
     </sheetView>
   </sheetViews>
@@ -21911,18 +21911,18 @@
       <c r="C2" t="s">
         <v>87</v>
       </c>
-      <c r="J2" s="45" t="s">
+      <c r="J2" s="51" t="s">
         <v>91</v>
       </c>
-      <c r="K2" s="46"/>
-      <c r="L2" s="46"/>
-      <c r="M2" s="47"/>
-      <c r="N2" s="48" t="s">
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="O2" s="46"/>
-      <c r="P2" s="46"/>
-      <c r="Q2" s="47"/>
+      <c r="O2" s="52"/>
+      <c r="P2" s="52"/>
+      <c r="Q2" s="53"/>
     </row>
     <row r="3" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -21937,25 +21937,25 @@
       <c r="J3" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="K3" s="43" t="s">
+      <c r="K3" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="L3" s="43" t="s">
+      <c r="L3" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="M3" s="44" t="s">
+      <c r="M3" s="46" t="s">
         <v>90</v>
       </c>
       <c r="N3" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="O3" s="43" t="s">
+      <c r="O3" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="P3" s="43" t="s">
+      <c r="P3" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="Q3" s="44" t="s">
+      <c r="Q3" s="46" t="s">
         <v>90</v>
       </c>
     </row>
@@ -21963,15 +21963,15 @@
       <c r="J4" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="44"/>
+      <c r="K4" s="45"/>
+      <c r="L4" s="45"/>
+      <c r="M4" s="46"/>
       <c r="N4" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="44"/>
+      <c r="O4" s="45"/>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="46"/>
     </row>
     <row r="5" spans="3:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J5" s="22">
@@ -22268,82 +22268,82 @@
     </row>
     <row r="16" spans="3:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="10:21" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="J17" s="45" t="s">
+      <c r="J17" s="51" t="s">
         <v>96</v>
       </c>
-      <c r="K17" s="46"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="47"/>
-      <c r="N17" s="45" t="s">
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="51" t="s">
         <v>97</v>
       </c>
-      <c r="O17" s="46"/>
-      <c r="P17" s="46"/>
-      <c r="Q17" s="47"/>
-      <c r="R17" s="48" t="s">
+      <c r="O17" s="52"/>
+      <c r="P17" s="52"/>
+      <c r="Q17" s="53"/>
+      <c r="R17" s="54" t="s">
         <v>98</v>
       </c>
-      <c r="S17" s="46"/>
-      <c r="T17" s="46"/>
-      <c r="U17" s="47"/>
+      <c r="S17" s="52"/>
+      <c r="T17" s="52"/>
+      <c r="U17" s="53"/>
     </row>
     <row r="18" spans="10:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J18" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="K18" s="50" t="s">
+      <c r="K18" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="L18" s="53" t="s">
+      <c r="L18" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="M18" s="51" t="s">
+      <c r="M18" s="50" t="s">
         <v>90</v>
       </c>
       <c r="N18" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="O18" s="50" t="s">
+      <c r="O18" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="P18" s="53" t="s">
+      <c r="P18" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="Q18" s="51" t="s">
+      <c r="Q18" s="50" t="s">
         <v>90</v>
       </c>
       <c r="R18" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="S18" s="50" t="s">
+      <c r="S18" s="47" t="s">
         <v>103</v>
       </c>
-      <c r="T18" s="53" t="s">
+      <c r="T18" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="U18" s="51" t="s">
+      <c r="U18" s="50" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="19" spans="10:21" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J19" s="49" t="s">
+      <c r="J19" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="K19" s="50"/>
-      <c r="L19" s="54"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="49" t="s">
+      <c r="K19" s="47"/>
+      <c r="L19" s="49"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="37" t="s">
         <v>92</v>
       </c>
-      <c r="O19" s="50"/>
-      <c r="P19" s="54"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="52" t="s">
+      <c r="O19" s="47"/>
+      <c r="P19" s="49"/>
+      <c r="Q19" s="50"/>
+      <c r="R19" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="S19" s="50"/>
-      <c r="T19" s="54"/>
-      <c r="U19" s="51"/>
+      <c r="S19" s="47"/>
+      <c r="T19" s="49"/>
+      <c r="U19" s="50"/>
     </row>
     <row r="20" spans="10:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="J20" s="22">
@@ -22545,11 +22545,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="P3:P4"/>
-    <mergeCell ref="Q3:Q4"/>
-    <mergeCell ref="S18:S19"/>
-    <mergeCell ref="T18:T19"/>
     <mergeCell ref="U18:U19"/>
     <mergeCell ref="J2:M2"/>
     <mergeCell ref="N2:Q2"/>
@@ -22565,6 +22560,11 @@
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
     <mergeCell ref="M3:M4"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="P3:P4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="S18:S19"/>
+    <mergeCell ref="T18:T19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -22572,7 +22572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
@@ -23602,7 +23602,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -23869,7 +23869,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A6:V50"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -23880,18 +23880,18 @@
   <sheetData>
     <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="G6" s="2"/>
-      <c r="H6" s="40" t="s">
+      <c r="H6" s="42" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="40"/>
-      <c r="J6" s="40" t="s">
+      <c r="I6" s="42"/>
+      <c r="J6" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="40"/>
-      <c r="L6" s="40" t="s">
+      <c r="K6" s="42"/>
+      <c r="L6" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="40"/>
+      <c r="M6" s="42"/>
     </row>
     <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="D7" t="s">
@@ -24225,18 +24225,18 @@
         <v>8</v>
       </c>
       <c r="P15" s="17"/>
-      <c r="Q15" s="41">
+      <c r="Q15" s="43">
         <v>20</v>
       </c>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42">
+      <c r="R15" s="44"/>
+      <c r="S15" s="44">
         <v>24</v>
       </c>
-      <c r="T15" s="42"/>
-      <c r="U15" s="42">
+      <c r="T15" s="44"/>
+      <c r="U15" s="44">
         <v>28</v>
       </c>
-      <c r="V15" s="42"/>
+      <c r="V15" s="44"/>
     </row>
     <row r="16" spans="2:22" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
@@ -25079,7 +25079,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -25487,7 +25487,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26104,7 +26104,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -26116,7 +26116,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A2:A29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -26261,7 +26261,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:R43"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">

</xml_diff>